<commit_message>
Correção expo, Desvio Padrão e Revalidação Ok
</commit_message>
<xml_diff>
--- a/Validações Restaurante Sem Garçom/teste T e F - Fila Balcao.xlsx
+++ b/Validações Restaurante Sem Garçom/teste T e F - Fila Balcao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gian\Google Drive\Documentos\UNISINOS\2021-1\Simulacao e Modelagem de Sistemas\TGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8121A2-D63E-4F8B-B16F-0CDE194AC660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1BDE74-9C6E-4BF6-B5F3-9915211B309B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teste normal" sheetId="1" r:id="rId1"/>
@@ -6012,14 +6012,14 @@
       <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="12" max="12" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="17">
         <v>14.42371874</v>
       </c>
@@ -6042,7 +6042,7 @@
       <c r="Q1" s="53"/>
       <c r="R1" s="53"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>20.272395499999998</v>
       </c>
@@ -6063,7 +6063,7 @@
       <c r="Q2" s="53"/>
       <c r="R2" s="53"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>16.126547550000002</v>
       </c>
@@ -6086,7 +6086,7 @@
       <c r="Q3" s="53"/>
       <c r="R3" s="53"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>9.1676403549999996</v>
       </c>
@@ -6107,7 +6107,7 @@
       <c r="Q4" s="53"/>
       <c r="R4" s="53"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>6.6220501799999996</v>
       </c>
@@ -6128,7 +6128,7 @@
       <c r="Q5" s="53"/>
       <c r="R5" s="53"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>11.02301879</v>
       </c>
@@ -6149,7 +6149,7 @@
       <c r="Q6" s="53"/>
       <c r="R6" s="53"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>7.0736561179999997</v>
       </c>
@@ -6170,7 +6170,7 @@
       <c r="Q7" s="53"/>
       <c r="R7" s="53"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>11.192431210000001</v>
       </c>
@@ -6191,7 +6191,7 @@
       <c r="Q8" s="53"/>
       <c r="R8" s="53"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>20.736204950000001</v>
       </c>
@@ -6213,7 +6213,7 @@
       <c r="Q9" s="53"/>
       <c r="R9" s="53"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>20.360238320000001</v>
       </c>
@@ -6234,7 +6234,7 @@
       <c r="Q10" s="53"/>
       <c r="R10" s="53"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>11.84624636</v>
       </c>
@@ -6255,7 +6255,7 @@
       <c r="Q11" s="53"/>
       <c r="R11" s="53"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>7.5258840820000001</v>
       </c>
@@ -6276,7 +6276,7 @@
       <c r="Q12" s="53"/>
       <c r="R12" s="53"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>11.898729810000001</v>
       </c>
@@ -6299,7 +6299,7 @@
       <c r="Q13" s="53"/>
       <c r="R13" s="53"/>
     </row>
-    <row r="14" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>10.03270058</v>
       </c>
@@ -6322,7 +6322,7 @@
       <c r="Q14" s="68"/>
       <c r="R14" s="68"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>10.903902929999999</v>
       </c>
@@ -6345,7 +6345,7 @@
       <c r="Q15" s="53"/>
       <c r="R15" s="53"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>6.1023358859999997</v>
       </c>
@@ -6368,7 +6368,7 @@
       <c r="Q16" s="53"/>
       <c r="R16" s="53"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>11.1727171</v>
       </c>
@@ -6389,7 +6389,7 @@
       <c r="Q17" s="53"/>
       <c r="R17" s="53"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>6.5301310509999997</v>
       </c>
@@ -6410,7 +6410,7 @@
       <c r="Q18" s="53"/>
       <c r="R18" s="53"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>18.606902229999999</v>
       </c>
@@ -6433,7 +6433,7 @@
       <c r="Q19" s="53"/>
       <c r="R19" s="53"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>17.709295310000002</v>
       </c>
@@ -6454,7 +6454,7 @@
       <c r="Q20" s="53"/>
       <c r="R20" s="53"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C21" s="53"/>
       <c r="D21" s="58"/>
       <c r="E21" s="53"/>
@@ -6472,7 +6472,7 @@
       <c r="Q21" s="53"/>
       <c r="R21" s="53"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C22" s="53"/>
       <c r="D22" s="53"/>
       <c r="E22" s="53"/>
@@ -6490,7 +6490,7 @@
       <c r="Q22" s="53"/>
       <c r="R22" s="53"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C23" s="53"/>
       <c r="D23" s="53"/>
       <c r="E23" s="53"/>
@@ -6508,7 +6508,7 @@
       <c r="Q23" s="53"/>
       <c r="R23" s="53"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C24" s="53"/>
       <c r="D24" s="53"/>
       <c r="E24" s="53"/>
@@ -6526,7 +6526,7 @@
       <c r="Q24" s="53"/>
       <c r="R24" s="53"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D25" s="66" t="s">
         <v>46</v>
       </c>
@@ -6567,20 +6567,20 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <f>'teste T'!A16</f>
         <v>1.0666666666666667</v>
@@ -6593,7 +6593,7 @@
       </c>
       <c r="D2" s="69"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <f>'teste T'!B16</f>
         <v>0.26666666666666666</v>
@@ -6604,12 +6604,12 @@
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
@@ -6621,12 +6621,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E14" s="7" t="s">
         <v>1</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>11.2328845339</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -6699,7 +6699,7 @@
         <v>17.874684313710077</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" s="7" t="s">
         <v>6</v>
       </c>
@@ -6724,7 +6724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" s="7" t="s">
         <v>22</v>
       </c>
@@ -6733,7 +6733,7 @@
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" s="7" t="s">
         <v>23</v>
       </c>
@@ -6742,7 +6742,7 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="8" t="s">
         <v>24</v>
       </c>
@@ -6751,7 +6751,7 @@
       </c>
       <c r="G20" s="8"/>
     </row>
-    <row r="25" spans="5:10" ht="21" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:10" ht="21" x14ac:dyDescent="0.35">
       <c r="I25" t="s">
         <v>50</v>
       </c>
@@ -6759,47 +6759,47 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
       <c r="G29" s="39"/>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -6824,27 +6824,27 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="30.1796875" customWidth="1"/>
-    <col min="12" max="12" width="18.1796875" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="26.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A5" s="19">
         <v>1</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>3</v>
       </c>
@@ -6890,16 +6890,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>2</v>
       </c>
       <c r="B7" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f>ABS(media_a  - media_b)</f>
-        <v>0.4</v>
+        <v>0.20000000000000007</v>
       </c>
       <c r="F7">
         <f>10*10*(10+10-2)</f>
@@ -6913,7 +6913,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>0</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>11.2328845339</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>0</v>
       </c>
@@ -6955,16 +6955,16 @@
         <v>17.874684313710077</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>0</v>
       </c>
       <c r="B10" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <f>D7/D8</f>
-        <v>0.11547005383792516</v>
+        <v>5.7735026918962602E-2</v>
       </c>
       <c r="F10">
         <f>SQRT(F7/F8)</f>
@@ -6975,7 +6975,7 @@
       </c>
       <c r="H10" s="67">
         <f>D10*F10</f>
-        <v>1.0954451150103324</v>
+        <v>0.54772255750516641</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>3</v>
@@ -6987,12 +6987,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>1</v>
       </c>
       <c r="B11" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>4</v>
@@ -7002,12 +7002,12 @@
       </c>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>1</v>
       </c>
       <c r="B12" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>13</v>
@@ -7023,12 +7023,12 @@
       </c>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19">
         <v>0</v>
       </c>
       <c r="B13" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>12</v>
@@ -7044,12 +7044,12 @@
       </c>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A14" s="19">
         <v>0</v>
       </c>
       <c r="B14" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>52</v>
@@ -7062,14 +7062,14 @@
       </c>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f>AVERAGE(A5:A14)</f>
         <v>0.8</v>
       </c>
       <c r="B15" s="12">
         <f>AVERAGE(B5:B14)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>8</v>
@@ -7079,7 +7079,7 @@
       </c>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <f>_xlfn.VAR.S(A5:A14)</f>
         <v>1.0666666666666667</v>
@@ -7099,7 +7099,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>SQRT(A16)</f>
         <v>1.0327955589886444</v>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <f>(A5-media_a)^2</f>
         <v>3.999999999999998E-2</v>
@@ -7129,13 +7129,13 @@
       </c>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <f t="shared" ref="A19:A27" si="0">(A6-media_a)^2</f>
         <v>4.8400000000000007</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <f t="shared" si="0"/>
         <v>1.44</v>
@@ -7150,13 +7150,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="13">
         <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
@@ -7165,7 +7165,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
@@ -7174,25 +7174,25 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <f t="shared" si="0"/>
         <v>3.999999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <f t="shared" si="0"/>
         <v>3.999999999999998E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
@@ -7201,13 +7201,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>SUM(A18:A27)/9</f>
         <v>1.0666666666666669</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="32" t="s">
         <v>46</v>
       </c>
@@ -7233,12 +7233,12 @@
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="9.6328125" customWidth="1"/>
+    <col min="5" max="6" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -7412,7 +7412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
@@ -7456,7 +7456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>11</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>12</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>13</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>14</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>15</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>16</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>17</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>18</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>19</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>20</v>
       </c>
@@ -7618,7 +7618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>21</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>22</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>23</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>24</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>25</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>26</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>27</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>28</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>29</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>30</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>31</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>32</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>33</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>34</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>35</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>36</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>37</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>38</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>39</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>40</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>41</v>
       </c>
@@ -7912,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>42</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>43</v>
       </c>
@@ -7940,7 +7940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>44</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>45</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>46</v>
       </c>
@@ -7982,7 +7982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>47</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>48</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>49</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>50</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>51</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>52</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>53</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>54</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>55</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>56</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>57</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>58</v>
       </c>
@@ -8150,7 +8150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>59</v>
       </c>
@@ -8164,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>60</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>61</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>62</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>63</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>64</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>65</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>66</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>67</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>68</v>
       </c>
@@ -8290,7 +8290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>69</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>70</v>
       </c>
@@ -8318,7 +8318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>71</v>
       </c>
@@ -8332,7 +8332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>72</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>73</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>74</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>75</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>76</v>
       </c>
@@ -8402,7 +8402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>77</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>78</v>
       </c>
@@ -8430,7 +8430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>79</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>80</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>81</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>82</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>83</v>
       </c>
@@ -8500,7 +8500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>84</v>
       </c>
@@ -8514,7 +8514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>85</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>86</v>
       </c>
@@ -8542,7 +8542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>87</v>
       </c>
@@ -8556,7 +8556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>88</v>
       </c>
@@ -8570,7 +8570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>89</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>90</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>91</v>
       </c>
@@ -8612,7 +8612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>92</v>
       </c>
@@ -8626,7 +8626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>93</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>94</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>95</v>
       </c>
@@ -8668,7 +8668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>96</v>
       </c>
@@ -8682,7 +8682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>97</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>98</v>
       </c>
@@ -8710,7 +8710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>99</v>
       </c>
@@ -8724,7 +8724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>100</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>101</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>102</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>103</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>104</v>
       </c>
@@ -8794,7 +8794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>105</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>106</v>
       </c>
@@ -8822,7 +8822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>107</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>108</v>
       </c>
@@ -8850,7 +8850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>109</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>110</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>111</v>
       </c>
@@ -8892,7 +8892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>112</v>
       </c>
@@ -8906,7 +8906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>113</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>114</v>
       </c>
@@ -8934,7 +8934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>115</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>116</v>
       </c>
@@ -8962,7 +8962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>117</v>
       </c>
@@ -8976,7 +8976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>118</v>
       </c>
@@ -8990,7 +8990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>119</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>120</v>
       </c>
@@ -9018,7 +9018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>121</v>
       </c>
@@ -9032,7 +9032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>122</v>
       </c>
@@ -9046,7 +9046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>123</v>
       </c>
@@ -9060,7 +9060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>124</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>125</v>
       </c>
@@ -9088,7 +9088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>126</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>127</v>
       </c>
@@ -9116,7 +9116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>128</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B130">
         <v>129</v>
       </c>
@@ -9144,7 +9144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B131">
         <v>130</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B132">
         <v>131</v>
       </c>
@@ -9172,7 +9172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B133">
         <v>132</v>
       </c>
@@ -9186,7 +9186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B134">
         <v>133</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B135">
         <v>134</v>
       </c>
@@ -9214,7 +9214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136">
         <v>135</v>
       </c>
@@ -9228,7 +9228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B137">
         <v>136</v>
       </c>
@@ -9242,7 +9242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>137</v>
       </c>
@@ -9256,7 +9256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B139">
         <v>138</v>
       </c>
@@ -9270,7 +9270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>139</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141">
         <v>140</v>
       </c>
@@ -9298,7 +9298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B142">
         <v>141</v>
       </c>
@@ -9312,7 +9312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>142</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>143</v>
       </c>
@@ -9340,7 +9340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B145">
         <v>144</v>
       </c>
@@ -9354,7 +9354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B146">
         <v>145</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B147">
         <v>146</v>
       </c>
@@ -9382,7 +9382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B148">
         <v>147</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B149">
         <v>148</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B150">
         <v>149</v>
       </c>
@@ -9424,7 +9424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B151">
         <v>150</v>
       </c>
@@ -9438,7 +9438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B152">
         <v>151</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B153">
         <v>152</v>
       </c>
@@ -9466,7 +9466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B154">
         <v>153</v>
       </c>
@@ -9480,7 +9480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B155">
         <v>154</v>
       </c>
@@ -9494,7 +9494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B156">
         <v>155</v>
       </c>
@@ -9508,7 +9508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B157">
         <v>156</v>
       </c>
@@ -9522,7 +9522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B158">
         <v>157</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B159">
         <v>158</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B160">
         <v>159</v>
       </c>
@@ -9564,7 +9564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B161">
         <v>160</v>
       </c>
@@ -9578,7 +9578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B162">
         <v>161</v>
       </c>
@@ -9592,7 +9592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B163">
         <v>162</v>
       </c>
@@ -9606,7 +9606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B164">
         <v>163</v>
       </c>
@@ -9620,7 +9620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B165">
         <v>164</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B166">
         <v>165</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B167">
         <v>166</v>
       </c>
@@ -9662,7 +9662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B168">
         <v>167</v>
       </c>
@@ -9676,7 +9676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B169">
         <v>168</v>
       </c>
@@ -9690,7 +9690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B170">
         <v>169</v>
       </c>
@@ -9704,7 +9704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B171">
         <v>170</v>
       </c>
@@ -9718,7 +9718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B172">
         <v>171</v>
       </c>
@@ -9732,7 +9732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B173">
         <v>172</v>
       </c>
@@ -9746,7 +9746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B174">
         <v>173</v>
       </c>
@@ -9760,7 +9760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B175">
         <v>174</v>
       </c>
@@ -9774,7 +9774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B176">
         <v>175</v>
       </c>
@@ -9788,7 +9788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B177">
         <v>176</v>
       </c>
@@ -9802,7 +9802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>177</v>
       </c>
@@ -9816,7 +9816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B179">
         <v>178</v>
       </c>
@@ -9830,7 +9830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>179</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B181">
         <v>180</v>
       </c>
@@ -9858,7 +9858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>181</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B183">
         <v>182</v>
       </c>
@@ -9886,7 +9886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>183</v>
       </c>
@@ -9900,7 +9900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>184</v>
       </c>
@@ -9914,7 +9914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>185</v>
       </c>
@@ -9928,7 +9928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B187">
         <v>186</v>
       </c>
@@ -9942,7 +9942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>187</v>
       </c>
@@ -9956,7 +9956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B189">
         <v>188</v>
       </c>
@@ -9970,7 +9970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B190">
         <v>189</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>190</v>
       </c>
@@ -9998,7 +9998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>191</v>
       </c>
@@ -10012,7 +10012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B193">
         <v>192</v>
       </c>
@@ -10026,7 +10026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B194">
         <v>193</v>
       </c>
@@ -10040,7 +10040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B195">
         <v>194</v>
       </c>
@@ -10054,7 +10054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B196">
         <v>195</v>
       </c>
@@ -10068,7 +10068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B197">
         <v>196</v>
       </c>
@@ -10082,7 +10082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B198">
         <v>197</v>
       </c>
@@ -10096,7 +10096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B199">
         <v>198</v>
       </c>
@@ -10110,7 +10110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B200">
         <v>199</v>
       </c>
@@ -10124,7 +10124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B201">
         <v>200</v>
       </c>
@@ -10138,7 +10138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B202">
         <v>201</v>
       </c>
@@ -10152,7 +10152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B203">
         <v>202</v>
       </c>
@@ -10166,7 +10166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B204">
         <v>203</v>
       </c>
@@ -10180,7 +10180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B205">
         <v>204</v>
       </c>
@@ -10194,7 +10194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B206">
         <v>205</v>
       </c>
@@ -10208,7 +10208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B207">
         <v>206</v>
       </c>
@@ -10222,7 +10222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B208">
         <v>207</v>
       </c>
@@ -10236,7 +10236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B209">
         <v>208</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B210">
         <v>209</v>
       </c>
@@ -10264,7 +10264,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B211">
         <v>210</v>
       </c>
@@ -10278,7 +10278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B212">
         <v>211</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B213">
         <v>212</v>
       </c>
@@ -10306,7 +10306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B214">
         <v>213</v>
       </c>
@@ -10320,7 +10320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B215">
         <v>214</v>
       </c>
@@ -10334,7 +10334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B216">
         <v>215</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B217">
         <v>216</v>
       </c>
@@ -10362,7 +10362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B218">
         <v>217</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B219">
         <v>218</v>
       </c>
@@ -10390,7 +10390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B220">
         <v>219</v>
       </c>
@@ -10398,7 +10398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B221">
         <v>220</v>
       </c>
@@ -10406,7 +10406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B222">
         <v>221</v>
       </c>
@@ -10414,7 +10414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B223">
         <v>222</v>
       </c>
@@ -10422,7 +10422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B224">
         <v>223</v>
       </c>
@@ -10430,7 +10430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225">
         <v>224</v>
       </c>
@@ -10438,7 +10438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226">
         <v>225</v>
       </c>
@@ -10446,7 +10446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227">
         <v>226</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228">
         <v>227</v>
       </c>
@@ -10462,7 +10462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229">
         <v>228</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230">
         <v>229</v>
       </c>
@@ -10478,7 +10478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231">
         <v>230</v>
       </c>
@@ -10486,7 +10486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232">
         <v>231</v>
       </c>
@@ -10494,7 +10494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233">
         <v>232</v>
       </c>
@@ -10502,7 +10502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234">
         <v>233</v>
       </c>
@@ -10510,7 +10510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235">
         <v>234</v>
       </c>
@@ -10518,7 +10518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236">
         <v>235</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237">
         <v>236</v>
       </c>
@@ -10534,7 +10534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238">
         <v>237</v>
       </c>
@@ -10542,7 +10542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239">
         <v>238</v>
       </c>
@@ -10550,7 +10550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240">
         <v>239</v>
       </c>
@@ -10558,7 +10558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B241">
         <v>240</v>
       </c>
@@ -10566,7 +10566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B242">
         <v>241</v>
       </c>
@@ -10574,7 +10574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B243">
         <v>242</v>
       </c>
@@ -10582,7 +10582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B244">
         <v>243</v>
       </c>
@@ -10590,7 +10590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B245">
         <v>244</v>
       </c>
@@ -10598,7 +10598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B246">
         <v>245</v>
       </c>
@@ -10606,7 +10606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247">
         <v>246</v>
       </c>
@@ -10614,7 +10614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B248">
         <v>247</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B249">
         <v>248</v>
       </c>
@@ -10630,7 +10630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B250">
         <v>249</v>
       </c>
@@ -10638,7 +10638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B251">
         <v>250</v>
       </c>
@@ -10646,7 +10646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B252">
         <v>251</v>
       </c>
@@ -10654,7 +10654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B253">
         <v>252</v>
       </c>
@@ -10662,7 +10662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B254">
         <v>253</v>
       </c>
@@ -10670,7 +10670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B255">
         <v>254</v>
       </c>
@@ -10678,7 +10678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B256">
         <v>255</v>
       </c>
@@ -10686,7 +10686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B257">
         <v>256</v>
       </c>
@@ -10694,7 +10694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B258">
         <v>257</v>
       </c>
@@ -10702,7 +10702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B259">
         <v>258</v>
       </c>
@@ -10710,7 +10710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B260">
         <v>259</v>
       </c>
@@ -10718,7 +10718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B261">
         <v>260</v>
       </c>
@@ -10726,7 +10726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B262">
         <v>261</v>
       </c>
@@ -10734,7 +10734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B263">
         <v>262</v>
       </c>
@@ -10742,7 +10742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B264">
         <v>263</v>
       </c>
@@ -10750,7 +10750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B265">
         <v>264</v>
       </c>
@@ -10758,7 +10758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B266">
         <v>265</v>
       </c>
@@ -10766,7 +10766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B267">
         <v>266</v>
       </c>
@@ -10774,7 +10774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B268">
         <v>267</v>
       </c>
@@ -10782,7 +10782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B269">
         <v>268</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B270">
         <v>269</v>
       </c>
@@ -10798,7 +10798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B271">
         <v>270</v>
       </c>
@@ -10806,7 +10806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B272">
         <v>271</v>
       </c>
@@ -10814,7 +10814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B273">
         <v>272</v>
       </c>
@@ -10822,7 +10822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B274">
         <v>273</v>
       </c>
@@ -10830,7 +10830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B275">
         <v>274</v>
       </c>
@@ -10838,7 +10838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B276">
         <v>275</v>
       </c>
@@ -10846,7 +10846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B277">
         <v>276</v>
       </c>
@@ -10854,7 +10854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B278">
         <v>277</v>
       </c>
@@ -10862,7 +10862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B279">
         <v>278</v>
       </c>
@@ -10870,7 +10870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B280">
         <v>279</v>
       </c>
@@ -10878,7 +10878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B281">
         <v>280</v>
       </c>
@@ -10886,7 +10886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B282">
         <v>281</v>
       </c>
@@ -10894,7 +10894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B283">
         <v>282</v>
       </c>
@@ -10902,7 +10902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B284">
         <v>283</v>
       </c>
@@ -10910,7 +10910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B285">
         <v>284</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B286">
         <v>285</v>
       </c>
@@ -10926,7 +10926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="287" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B287">
         <v>286</v>
       </c>
@@ -10934,7 +10934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="288" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B288">
         <v>287</v>
       </c>
@@ -10942,7 +10942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B289">
         <v>288</v>
       </c>
@@ -10950,7 +10950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290">
         <v>289</v>
       </c>
@@ -10958,7 +10958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291">
         <v>290</v>
       </c>
@@ -10966,7 +10966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292">
         <v>291</v>
       </c>
@@ -10974,7 +10974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293">
         <v>292</v>
       </c>
@@ -10982,7 +10982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294">
         <v>293</v>
       </c>
@@ -10990,7 +10990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295">
         <v>294</v>
       </c>
@@ -10998,7 +10998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296">
         <v>295</v>
       </c>
@@ -11006,7 +11006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297">
         <v>296</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298">
         <v>297</v>
       </c>
@@ -11022,7 +11022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299">
         <v>298</v>
       </c>
@@ -11030,7 +11030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300">
         <v>299</v>
       </c>
@@ -11038,7 +11038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301">
         <v>300</v>
       </c>
@@ -11046,7 +11046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302">
         <v>301</v>
       </c>
@@ -11054,7 +11054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303">
         <v>302</v>
       </c>
@@ -11062,7 +11062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304">
         <v>303</v>
       </c>
@@ -11070,7 +11070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305">
         <v>304</v>
       </c>
@@ -11078,7 +11078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306">
         <v>305</v>
       </c>
@@ -11086,7 +11086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307">
         <v>306</v>
       </c>
@@ -11094,7 +11094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308">
         <v>307</v>
       </c>
@@ -11102,7 +11102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309">
         <v>308</v>
       </c>
@@ -11110,7 +11110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310">
         <v>309</v>
       </c>
@@ -11118,7 +11118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311">
         <v>310</v>
       </c>
@@ -11126,7 +11126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312">
         <v>311</v>
       </c>
@@ -11134,7 +11134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313">
         <v>312</v>
       </c>
@@ -11142,7 +11142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314">
         <v>313</v>
       </c>
@@ -11150,7 +11150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315">
         <v>314</v>
       </c>
@@ -11158,7 +11158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316">
         <v>315</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317">
         <v>316</v>
       </c>
@@ -11174,7 +11174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318">
         <v>317</v>
       </c>
@@ -11182,7 +11182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319">
         <v>318</v>
       </c>
@@ -11190,7 +11190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320">
         <v>319</v>
       </c>
@@ -11198,7 +11198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321">
         <v>320</v>
       </c>
@@ -11206,7 +11206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322">
         <v>321</v>
       </c>
@@ -11214,7 +11214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323">
         <v>322</v>
       </c>
@@ -11222,7 +11222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324">
         <v>323</v>
       </c>
@@ -11230,7 +11230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325">
         <v>324</v>
       </c>
@@ -11238,7 +11238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326">
         <v>325</v>
       </c>
@@ -11246,7 +11246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327">
         <v>326</v>
       </c>
@@ -11254,7 +11254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328">
         <v>327</v>
       </c>
@@ -11262,7 +11262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329">
         <v>328</v>
       </c>
@@ -11270,7 +11270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330">
         <v>329</v>
       </c>
@@ -11278,7 +11278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331">
         <v>330</v>
       </c>
@@ -11286,7 +11286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332">
         <v>331</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333">
         <v>332</v>
       </c>
@@ -11302,7 +11302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334">
         <v>333</v>
       </c>
@@ -11310,7 +11310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335">
         <v>334</v>
       </c>
@@ -11318,7 +11318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336">
         <v>335</v>
       </c>
@@ -11326,7 +11326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="337" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B337">
         <v>336</v>
       </c>
@@ -11334,7 +11334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="338" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B338">
         <v>337</v>
       </c>
@@ -11342,7 +11342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="339" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B339">
         <v>338</v>
       </c>
@@ -11350,7 +11350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="340" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B340">
         <v>339</v>
       </c>
@@ -11358,7 +11358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="341" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B341">
         <v>340</v>
       </c>
@@ -11366,7 +11366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="342" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B342">
         <v>341</v>
       </c>
@@ -11374,7 +11374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="343" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B343">
         <v>342</v>
       </c>
@@ -11382,7 +11382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="344" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B344">
         <v>343</v>
       </c>
@@ -11390,7 +11390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="345" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B345">
         <v>344</v>
       </c>
@@ -11398,7 +11398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="346" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B346">
         <v>345</v>
       </c>
@@ -11406,7 +11406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B347">
         <v>346</v>
       </c>
@@ -11414,7 +11414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="348" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B348">
         <v>347</v>
       </c>
@@ -11422,7 +11422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="349" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B349">
         <v>348</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B350">
         <v>349</v>
       </c>
@@ -11438,7 +11438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B351">
         <v>350</v>
       </c>
@@ -11446,7 +11446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="352" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B352">
         <v>351</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="353" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B353">
         <v>352</v>
       </c>
@@ -11462,7 +11462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B354">
         <v>353</v>
       </c>
@@ -11470,7 +11470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="355" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B355">
         <v>354</v>
       </c>
@@ -11478,7 +11478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="356" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B356">
         <v>355</v>
       </c>
@@ -11486,7 +11486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="357" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B357">
         <v>356</v>
       </c>
@@ -11494,7 +11494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="358" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B358">
         <v>357</v>
       </c>
@@ -11502,7 +11502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="359" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B359">
         <v>358</v>
       </c>
@@ -11510,7 +11510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="360" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B360">
         <v>359</v>
       </c>
@@ -11518,7 +11518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="361" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B361">
         <v>360</v>
       </c>
@@ -11526,7 +11526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="362" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B362">
         <v>361</v>
       </c>
@@ -11534,7 +11534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="363" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B363">
         <v>362</v>
       </c>
@@ -11542,7 +11542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="364" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B364">
         <v>363</v>
       </c>
@@ -11550,7 +11550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="365" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B365">
         <v>364</v>
       </c>
@@ -11558,7 +11558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="366" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B366">
         <v>365</v>
       </c>
@@ -11566,7 +11566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="367" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B367">
         <v>366</v>
       </c>
@@ -11574,7 +11574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="368" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B368">
         <v>367</v>
       </c>
@@ -11582,7 +11582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369">
         <v>368</v>
       </c>
@@ -11590,7 +11590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370">
         <v>369</v>
       </c>
@@ -11598,7 +11598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371">
         <v>370</v>
       </c>
@@ -11606,7 +11606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372">
         <v>371</v>
       </c>
@@ -11614,7 +11614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373">
         <v>372</v>
       </c>
@@ -11622,7 +11622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374">
         <v>373</v>
       </c>
@@ -11630,7 +11630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375">
         <v>374</v>
       </c>
@@ -11638,7 +11638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376">
         <v>375</v>
       </c>
@@ -11646,7 +11646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377">
         <v>376</v>
       </c>
@@ -11654,7 +11654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="378" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378">
         <v>377</v>
       </c>
@@ -11662,7 +11662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379">
         <v>378</v>
       </c>
@@ -11670,7 +11670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="380" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380">
         <v>379</v>
       </c>
@@ -11678,7 +11678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381">
         <v>380</v>
       </c>
@@ -11686,7 +11686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="382" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382">
         <v>381</v>
       </c>
@@ -11694,7 +11694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="383" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383">
         <v>382</v>
       </c>
@@ -11702,7 +11702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384">
         <v>383</v>
       </c>
@@ -11710,7 +11710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="385" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B385">
         <v>384</v>
       </c>
@@ -11718,7 +11718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B386">
         <v>385</v>
       </c>
@@ -11726,7 +11726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="387" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B387">
         <v>386</v>
       </c>
@@ -11734,7 +11734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B388">
         <v>387</v>
       </c>
@@ -11742,7 +11742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B389">
         <v>388</v>
       </c>
@@ -11750,7 +11750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="390" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B390">
         <v>389</v>
       </c>
@@ -11758,7 +11758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="391" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B391">
         <v>390</v>
       </c>
@@ -11766,7 +11766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="392" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B392">
         <v>391</v>
       </c>
@@ -11774,7 +11774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B393">
         <v>392</v>
       </c>
@@ -11782,7 +11782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="394" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="394" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B394">
         <v>393</v>
       </c>
@@ -11790,7 +11790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="395" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B395">
         <v>394</v>
       </c>
@@ -11798,7 +11798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="396" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="396" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B396">
         <v>395</v>
       </c>
@@ -11806,7 +11806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="397" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="397" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B397">
         <v>396</v>
       </c>
@@ -11814,7 +11814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="398" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="398" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B398">
         <v>397</v>
       </c>
@@ -11822,7 +11822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="399" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="399" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B399">
         <v>398</v>
       </c>
@@ -11830,7 +11830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="400" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="400" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B400">
         <v>399</v>
       </c>
@@ -11838,7 +11838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="401" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B401">
         <v>400</v>
       </c>
@@ -11846,7 +11846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="402" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B402">
         <v>401</v>
       </c>
@@ -11854,7 +11854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="403" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403">
         <v>402</v>
       </c>
@@ -11862,7 +11862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="404" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404">
         <v>403</v>
       </c>
@@ -11870,7 +11870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="405" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="405" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B405">
         <v>404</v>
       </c>
@@ -11878,7 +11878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="406" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406">
         <v>405</v>
       </c>
@@ -11886,7 +11886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="407" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407">
         <v>406</v>
       </c>
@@ -11894,7 +11894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="408" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408">
         <v>407</v>
       </c>
@@ -11902,7 +11902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="409" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409">
         <v>408</v>
       </c>
@@ -11910,7 +11910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="410" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410">
         <v>409</v>
       </c>
@@ -11918,7 +11918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="411" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411">
         <v>410</v>
       </c>
@@ -11926,7 +11926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="412" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412">
         <v>411</v>
       </c>
@@ -11934,7 +11934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="413" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413">
         <v>412</v>
       </c>
@@ -11942,7 +11942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="414" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="414" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B414">
         <v>413</v>
       </c>
@@ -11950,7 +11950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="415" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415">
         <v>414</v>
       </c>
@@ -11958,7 +11958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="416" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416">
         <v>415</v>
       </c>
@@ -11966,7 +11966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="417" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417">
         <v>416</v>
       </c>
@@ -11974,7 +11974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="418" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418">
         <v>417</v>
       </c>
@@ -11982,7 +11982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="419" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419">
         <v>418</v>
       </c>
@@ -12007,12 +12007,12 @@
       <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -12020,7 +12020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -12028,7 +12028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -12037,16 +12037,16 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="45">
         <f>media_b</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -12055,7 +12055,7 @@
         <v>1.0666666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -12064,7 +12064,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -12080,47 +12080,47 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>(B6/10)^2/9+(B7/10)^2/9</f>
         <v>1.3432098765432097E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>103</v>
       </c>
       <c r="B12">
         <f>B4-B5</f>
-        <v>0.4</v>
+        <v>0.20000000000000007</v>
       </c>
       <c r="C12" s="5">
         <f>B12/B13</f>
-        <v>1.0954451150103324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.5477225575051663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SQRT(B6/10+B7/10)</f>
         <v>0.36514837167011072</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>87</v>
       </c>
@@ -12128,12 +12128,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A23" s="34" t="s">
         <v>85</v>
       </c>
@@ -12158,21 +12158,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="3.453125" customWidth="1"/>
-    <col min="7" max="7" width="4.81640625" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.7265625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
@@ -12189,7 +12189,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="40">
         <v>6.6220501799999996</v>
       </c>
@@ -12218,7 +12218,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="40">
         <v>7.0736561179999997</v>
       </c>
@@ -12247,7 +12247,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="40">
         <v>9.1676403549999996</v>
       </c>
@@ -12273,7 +12273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="40">
         <v>11.02301879</v>
       </c>
@@ -12299,7 +12299,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
         <v>11.192431210000001</v>
       </c>
@@ -12325,7 +12325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
         <v>14.42371874</v>
       </c>
@@ -12351,7 +12351,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>16.126547550000002</v>
       </c>
@@ -12377,7 +12377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <v>20.272395499999998</v>
       </c>
@@ -12403,7 +12403,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>20.360238320000001</v>
       </c>
@@ -12429,7 +12429,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>20.736204950000001</v>
       </c>
@@ -12455,7 +12455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E12" s="40">
         <v>11.192431210000001</v>
       </c>
@@ -12474,7 +12474,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="C13" s="63" t="s">
         <v>81</v>
       </c>
@@ -12501,7 +12501,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="E14" s="41">
         <v>11.898729810000001</v>
       </c>
@@ -12519,7 +12519,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E15" s="40">
         <v>14.42371874</v>
       </c>
@@ -12537,7 +12537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E16" s="40">
         <v>16.126547550000002</v>
       </c>
@@ -12550,7 +12550,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E17" s="41">
         <v>17.709295310000002</v>
       </c>
@@ -12568,7 +12568,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E18" s="41">
         <v>18.606902229999999</v>
       </c>
@@ -12593,7 +12593,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="5:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E19" s="40">
         <v>20.272395499999998</v>
       </c>
@@ -12611,7 +12611,7 @@
         <v>-1.0583005244258363</v>
       </c>
     </row>
-    <row r="20" spans="5:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="40">
         <v>20.360238320000001</v>
       </c>
@@ -12622,7 +12622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="5:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21" s="40">
         <v>20.736204950000001</v>
       </c>
@@ -12638,17 +12638,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
       <c r="I23" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
       <c r="I24" s="64" t="s">
         <v>93</v>
       </c>

</xml_diff>